<commit_message>
Revert "Merge branch 'main' of https://github.com/BeyonDog/GQLX"
This reverts commit 751e405986c793b3dc70357306d52788ead851a0, reversing
changes made to 790a66b8714bc4dab6b8300dcdb35a10ed98605e.
</commit_message>
<xml_diff>
--- a/DataTable/功能表.xlsx
+++ b/DataTable/功能表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubCangKu\GQLX\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05569E46-EAB8-463E-839F-34F44D8B4606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AD0BF8-3C31-47D6-9468-501B5DB3EFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>ALL</t>
   </si>
@@ -150,12 +150,18 @@
     <t>幸运值</t>
   </si>
   <si>
+    <t>HP</t>
+  </si>
+  <si>
     <t>生命值</t>
   </si>
   <si>
     <t>1,2</t>
   </si>
   <si>
+    <t>ZY#0109</t>
+  </si>
+  <si>
     <t>金币</t>
   </si>
   <si>
@@ -300,30 +306,6 @@
   </si>
   <si>
     <t>值</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZY#0101</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZY#0102</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZY#0103</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZY#0104</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>HP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZY#0109</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -644,7 +626,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -829,15 +811,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1125,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -1202,69 +1175,69 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="56" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D2" s="56" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H2" s="58" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I2" s="56" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J2" s="57" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K2" s="58" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L2" s="56" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M2" s="56" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N2" s="56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="O2" s="59" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P2" s="60" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Q2" s="59" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="R2" s="59" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>2</v>
@@ -1273,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>2</v>
@@ -1285,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="57" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>3</v>
@@ -1309,7 +1282,7 @@
         <v>3</v>
       </c>
       <c r="R3" s="59" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -1365,12 +1338,12 @@
         <v>21</v>
       </c>
       <c r="R4" s="61" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A5" s="62" t="s">
-        <v>74</v>
+      <c r="A5" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>23</v>
@@ -1401,8 +1374,8 @@
       <c r="R5" s="50"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A6" s="62" t="s">
-        <v>75</v>
+      <c r="A6" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>25</v>
@@ -1433,8 +1406,8 @@
       <c r="R6" s="50"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A7" s="62" t="s">
-        <v>76</v>
+      <c r="A7" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>27</v>
@@ -1465,8 +1438,8 @@
       <c r="R7" s="50"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A8" s="62" t="s">
-        <v>77</v>
+      <c r="A8" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>29</v>
@@ -1497,14 +1470,14 @@
       <c r="R8" s="50"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A9" s="63" t="s">
-        <v>78</v>
+      <c r="A9" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14">
         <v>1</v>
@@ -1524,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N9" s="37">
         <v>125125</v>
@@ -1535,14 +1508,14 @@
       <c r="R9" s="51"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A10" s="64" t="s">
-        <v>79</v>
+      <c r="A10" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>
@@ -1557,7 +1530,7 @@
         <v>50</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K10" s="19">
         <v>0</v>
@@ -1572,13 +1545,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D11" s="20">
         <v>2</v>
@@ -1593,7 +1566,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K11" s="22">
         <v>1</v>
@@ -1602,10 +1575,10 @@
         <v>22</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O11" s="42">
         <v>3</v>
@@ -1620,13 +1593,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D12" s="20">
         <v>2</v>
@@ -1641,7 +1614,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K12" s="22">
         <v>1</v>
@@ -1650,10 +1623,10 @@
         <v>22</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O12" s="42">
         <v>3</v>
@@ -1668,13 +1641,13 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13" s="20">
         <v>2</v>
@@ -1689,7 +1662,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K13" s="22">
         <v>1</v>
@@ -1698,10 +1671,10 @@
         <v>22</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O13" s="42">
         <v>3</v>
@@ -1716,13 +1689,13 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D14" s="20">
         <v>2</v>
@@ -1737,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K14" s="22">
         <v>1</v>
@@ -1746,10 +1719,10 @@
         <v>22</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O14" s="42">
         <v>3</v>
@@ -1764,13 +1737,13 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D15" s="23">
         <v>3</v>
@@ -1796,13 +1769,13 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="23">
         <v>3</v>
@@ -1828,13 +1801,13 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D17" s="23">
         <v>3</v>
@@ -1860,13 +1833,13 @@
     </row>
     <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D18" s="23">
         <v>3</v>

</xml_diff>